<commit_message>
implementatiestatus toegevoegd aan mapping
</commit_message>
<xml_diff>
--- a/transponering/mapping-deel-Gebouw-en-VBO.xlsx
+++ b/transponering/mapping-deel-Gebouw-en-VBO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\silfh\Dropbox\1 BGTservices\klanten\191101 (Geonovum)\team dis-geo\algemeen DIS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvandenbrink\Documents\github\disgeo-demo-3a\transponering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF70B810-5AE1-4B9D-A599-A7CDE7DF956C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A330104A-55EF-444E-9EB9-7F25424EA3D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5445" yWindow="3105" windowWidth="31425" windowHeight="16575" tabRatio="331" firstSheet="1" activeTab="4" xr2:uid="{FC9435B0-E85B-4538-B212-DC31D83D01A0}"/>
+    <workbookView xWindow="-38520" yWindow="-3825" windowWidth="38640" windowHeight="21240" tabRatio="331" xr2:uid="{FC9435B0-E85B-4538-B212-DC31D83D01A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Gebouw" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="340">
   <si>
     <t>Bedrijfsgebouw</t>
   </si>
@@ -1114,6 +1114,21 @@
   </si>
   <si>
     <t>in SOR model wordt aangegeven dat de geometrie een punt, een lijn of een vlak kan zijn. Uit BGT zijn het alleen punten.</t>
+  </si>
+  <si>
+    <t>deels geimplementeerd ivm scope keuze</t>
+  </si>
+  <si>
+    <t>BAG pand nil invullen</t>
+  </si>
+  <si>
+    <t>geimplementeerd</t>
+  </si>
+  <si>
+    <t>geimplementeerd (in code, configuratiesyntax nog in ontwikkeling)</t>
+  </si>
+  <si>
+    <t>niet in EMSO maar wel geimplementeerd</t>
   </si>
 </sst>
 </file>
@@ -1805,10 +1820,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA24D532-5941-4A9B-B168-F20D396FA9EF}">
-  <dimension ref="B2:J66"/>
+  <dimension ref="A2:J66"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1826,7 +1841,7 @@
     <col min="11" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C2" s="10" t="s">
         <v>52</v>
       </c>
@@ -1834,7 +1849,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="2:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C3" s="7" t="s">
         <v>55</v>
       </c>
@@ -1842,7 +1857,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" s="7" t="s">
         <v>30</v>
       </c>
@@ -1850,7 +1865,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" s="7" t="s">
         <v>51</v>
       </c>
@@ -1858,7 +1873,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C6" s="7" t="s">
         <v>53</v>
       </c>
@@ -1866,7 +1881,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C7" s="12" t="s">
         <v>49</v>
       </c>
@@ -1874,7 +1889,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C11" s="14" t="s">
         <v>32</v>
       </c>
@@ -1888,7 +1903,7 @@
       <c r="I11" s="18"/>
       <c r="J11" s="26"/>
     </row>
-    <row r="12" spans="2:10" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B12" s="19" t="s">
         <v>58</v>
       </c>
@@ -1917,7 +1932,10 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
+        <v>335</v>
+      </c>
       <c r="B13" s="9" t="s">
         <v>31</v>
       </c>
@@ -1930,7 +1948,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="14" spans="2:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
         <v>0</v>
       </c>
@@ -1941,7 +1959,7 @@
       <c r="F14" s="23"/>
       <c r="I14" s="7"/>
     </row>
-    <row r="15" spans="2:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C15" s="3" t="s">
         <v>2</v>
       </c>
@@ -1952,7 +1970,7 @@
       <c r="F15" s="23"/>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="2:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C16" s="3" t="s">
         <v>143</v>
       </c>
@@ -1963,7 +1981,7 @@
       <c r="F16" s="23"/>
       <c r="I16" s="7"/>
     </row>
-    <row r="17" spans="3:9" ht="63" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="63" x14ac:dyDescent="0.25">
       <c r="C17" s="3"/>
       <c r="D17" s="4" t="s">
         <v>158</v>
@@ -1984,7 +2002,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="18" spans="3:9" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C18" s="3" t="s">
         <v>4</v>
       </c>
@@ -1995,7 +2013,7 @@
       <c r="F18" s="23"/>
       <c r="I18" s="7"/>
     </row>
-    <row r="19" spans="3:9" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C19" s="3" t="s">
         <v>6</v>
       </c>
@@ -2006,7 +2024,7 @@
       <c r="F19" s="23"/>
       <c r="I19" s="7"/>
     </row>
-    <row r="20" spans="3:9" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C20" s="3" t="s">
         <v>8</v>
       </c>
@@ -2017,7 +2035,7 @@
       <c r="F20" s="23"/>
       <c r="I20" s="7"/>
     </row>
-    <row r="21" spans="3:9" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C21" s="3" t="s">
         <v>10</v>
       </c>
@@ -2028,7 +2046,7 @@
       <c r="F21" s="23"/>
       <c r="I21" s="7"/>
     </row>
-    <row r="22" spans="3:9" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C22" s="3" t="s">
         <v>12</v>
       </c>
@@ -2039,7 +2057,7 @@
       <c r="F22" s="23"/>
       <c r="I22" s="7"/>
     </row>
-    <row r="23" spans="3:9" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C23" s="3" t="s">
         <v>14</v>
       </c>
@@ -2050,7 +2068,7 @@
       <c r="F23" s="23"/>
       <c r="I23" s="7"/>
     </row>
-    <row r="24" spans="3:9" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C24" s="3" t="s">
         <v>16</v>
       </c>
@@ -2063,7 +2081,7 @@
       <c r="F24" s="23"/>
       <c r="I24" s="7"/>
     </row>
-    <row r="25" spans="3:9" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C25" s="3" t="s">
         <v>18</v>
       </c>
@@ -2075,7 +2093,7 @@
       <c r="H25" s="24"/>
       <c r="I25" s="7"/>
     </row>
-    <row r="26" spans="3:9" ht="63" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="63" x14ac:dyDescent="0.25">
       <c r="C26" s="3" t="s">
         <v>143</v>
       </c>
@@ -2098,7 +2116,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="27" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C27" s="3"/>
       <c r="D27" s="4" t="s">
         <v>144</v>
@@ -2108,7 +2126,7 @@
       <c r="H27" s="24"/>
       <c r="I27" s="7"/>
     </row>
-    <row r="28" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C28" s="3"/>
       <c r="D28" s="4" t="s">
         <v>145</v>
@@ -2118,7 +2136,7 @@
       <c r="H28" s="24"/>
       <c r="I28" s="7"/>
     </row>
-    <row r="29" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C29" s="3"/>
       <c r="D29" s="4"/>
       <c r="E29" s="7"/>
@@ -2126,7 +2144,10 @@
       <c r="H29" s="24"/>
       <c r="I29" s="7"/>
     </row>
-    <row r="30" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="9" t="s">
+        <v>336</v>
+      </c>
       <c r="C30" s="5" t="s">
         <v>20</v>
       </c>
@@ -2137,17 +2158,20 @@
       <c r="F30" s="23"/>
       <c r="I30" s="7"/>
     </row>
-    <row r="31" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E31" s="7"/>
       <c r="F31" s="23"/>
       <c r="I31" s="7"/>
     </row>
-    <row r="32" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E32" s="7"/>
       <c r="F32" s="23"/>
       <c r="I32" s="7"/>
     </row>
-    <row r="33" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="9" t="s">
+        <v>228</v>
+      </c>
       <c r="B33" s="9" t="s">
         <v>35</v>
       </c>
@@ -2160,7 +2184,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="34" spans="2:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C34" s="1" t="s">
         <v>36</v>
       </c>
@@ -2171,7 +2195,7 @@
       <c r="F34" s="23"/>
       <c r="I34" s="7"/>
     </row>
-    <row r="35" spans="2:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C35" s="3" t="s">
         <v>38</v>
       </c>
@@ -2182,7 +2206,7 @@
       <c r="F35" s="23"/>
       <c r="I35" s="7"/>
     </row>
-    <row r="36" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C36" s="5" t="s">
         <v>40</v>
       </c>
@@ -2193,17 +2217,20 @@
       <c r="F36" s="23"/>
       <c r="I36" s="7"/>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E37" s="7"/>
       <c r="F37" s="23"/>
       <c r="I37" s="7"/>
     </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E38" s="7"/>
       <c r="F38" s="23"/>
       <c r="I38" s="7"/>
     </row>
-    <row r="39" spans="2:10" s="39" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" s="39" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A39" s="39" t="s">
+        <v>337</v>
+      </c>
       <c r="B39" s="38" t="s">
         <v>275</v>
       </c>
@@ -2226,7 +2253,10 @@
         <v>274</v>
       </c>
     </row>
-    <row r="40" spans="2:10" s="39" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="39" t="s">
+        <v>337</v>
+      </c>
       <c r="B40" s="38" t="s">
         <v>276</v>
       </c>
@@ -2249,7 +2279,10 @@
         <v>279</v>
       </c>
     </row>
-    <row r="41" spans="2:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A41" s="9" t="s">
+        <v>228</v>
+      </c>
       <c r="B41" s="25" t="s">
         <v>43</v>
       </c>
@@ -2265,7 +2298,10 @@
         <v>228</v>
       </c>
     </row>
-    <row r="42" spans="2:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A42" s="9" t="s">
+        <v>337</v>
+      </c>
       <c r="B42" s="25" t="s">
         <v>46</v>
       </c>
@@ -2285,7 +2321,10 @@
         <v>146</v>
       </c>
     </row>
-    <row r="43" spans="2:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A43" s="9" t="s">
+        <v>339</v>
+      </c>
       <c r="B43" s="25" t="s">
         <v>45</v>
       </c>
@@ -2305,7 +2344,10 @@
         <v>146</v>
       </c>
     </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="9" t="s">
+        <v>338</v>
+      </c>
       <c r="B44" s="38" t="s">
         <v>44</v>
       </c>
@@ -2324,7 +2366,7 @@
       <c r="I44" s="41"/>
       <c r="J44" s="43"/>
     </row>
-    <row r="45" spans="2:10" ht="63" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="B45" s="38"/>
       <c r="C45" s="39" t="s">
         <v>176</v>
@@ -2347,7 +2389,7 @@
       </c>
       <c r="J45" s="43"/>
     </row>
-    <row r="46" spans="2:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B46" s="38"/>
       <c r="C46" s="39" t="s">
         <v>178</v>
@@ -2370,7 +2412,7 @@
       </c>
       <c r="J46" s="43"/>
     </row>
-    <row r="47" spans="2:10" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
       <c r="B47" s="38"/>
       <c r="C47" s="39" t="s">
         <v>180</v>
@@ -2393,7 +2435,7 @@
       </c>
       <c r="J47" s="43"/>
     </row>
-    <row r="48" spans="2:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B48" s="38"/>
       <c r="C48" s="39" t="s">
         <v>182</v>
@@ -2576,7 +2618,7 @@
     <col min="11" max="16384" width="9.140625" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" s="31" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
@@ -2587,7 +2629,7 @@
       <c r="I1" s="9"/>
       <c r="J1" s="24"/>
     </row>
-    <row r="2" spans="2:10" s="31" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="9"/>
       <c r="C2" s="10" t="s">
         <v>52</v>
@@ -2602,7 +2644,7 @@
       <c r="I2" s="9"/>
       <c r="J2" s="24"/>
     </row>
-    <row r="3" spans="2:10" s="31" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="B3" s="9"/>
       <c r="C3" s="7"/>
       <c r="D3" s="11" t="s">
@@ -2615,7 +2657,7 @@
       <c r="I3" s="9"/>
       <c r="J3" s="24"/>
     </row>
-    <row r="4" spans="2:10" s="31" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="9"/>
       <c r="C4" s="7" t="s">
         <v>30</v>
@@ -2630,7 +2672,7 @@
       <c r="I4" s="9"/>
       <c r="J4" s="24"/>
     </row>
-    <row r="5" spans="2:10" s="31" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="9"/>
       <c r="C5" s="7" t="s">
         <v>51</v>
@@ -2643,7 +2685,7 @@
       <c r="I5" s="9"/>
       <c r="J5" s="24"/>
     </row>
-    <row r="6" spans="2:10" s="31" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="9"/>
       <c r="C6" s="7" t="s">
         <v>53</v>
@@ -2656,7 +2698,7 @@
       <c r="I6" s="9"/>
       <c r="J6" s="24"/>
     </row>
-    <row r="7" spans="2:10" s="31" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="9"/>
       <c r="C7" s="12" t="s">
         <v>49</v>
@@ -2669,7 +2711,7 @@
       <c r="I7" s="9"/>
       <c r="J7" s="24"/>
     </row>
-    <row r="8" spans="2:10" s="31" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
@@ -2680,7 +2722,7 @@
       <c r="I8" s="9"/>
       <c r="J8" s="24"/>
     </row>
-    <row r="9" spans="2:10" s="31" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
@@ -2691,7 +2733,7 @@
       <c r="I9" s="9"/>
       <c r="J9" s="24"/>
     </row>
-    <row r="10" spans="2:10" s="31" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
@@ -2702,7 +2744,7 @@
       <c r="I10" s="9"/>
       <c r="J10" s="24"/>
     </row>
-    <row r="11" spans="2:10" s="31" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="9"/>
       <c r="C11" s="14" t="s">
         <v>32</v>
@@ -2717,7 +2759,7 @@
       <c r="I11" s="18"/>
       <c r="J11" s="26"/>
     </row>
-    <row r="12" spans="2:10" s="31" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B12" s="19" t="s">
         <v>58</v>
       </c>
@@ -2746,49 +2788,35 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="2:10" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E13" s="51"/>
-      <c r="G13" s="35"/>
       <c r="I13" s="51"/>
-      <c r="J13" s="35"/>
-    </row>
-    <row r="14" spans="2:10" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E14" s="51"/>
-      <c r="G14" s="35"/>
       <c r="I14" s="51"/>
-      <c r="J14" s="35"/>
-    </row>
-    <row r="15" spans="2:10" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E15" s="51"/>
-      <c r="G15" s="35"/>
       <c r="I15" s="51"/>
-      <c r="J15" s="35"/>
-    </row>
-    <row r="16" spans="2:10" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E16" s="51"/>
-      <c r="G16" s="35"/>
       <c r="I16" s="51"/>
-      <c r="J16" s="35"/>
-    </row>
-    <row r="17" spans="2:10" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E17" s="51"/>
-      <c r="G17" s="35"/>
       <c r="I17" s="51"/>
-      <c r="J17" s="35"/>
-    </row>
-    <row r="18" spans="2:10" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E18" s="51"/>
-      <c r="G18" s="35"/>
       <c r="I18" s="51"/>
-      <c r="J18" s="35"/>
-    </row>
-    <row r="19" spans="2:10" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E19" s="51"/>
-      <c r="G19" s="35"/>
       <c r="I19" s="51"/>
-      <c r="J19" s="35"/>
-    </row>
-    <row r="20" spans="2:10" s="31" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="32" t="s">
         <v>67</v>
       </c>
@@ -2798,16 +2826,14 @@
       <c r="F20" s="32" t="s">
         <v>273</v>
       </c>
-      <c r="G20" s="35"/>
       <c r="H20" s="32" t="s">
         <v>198</v>
       </c>
       <c r="I20" s="51" t="s">
         <v>199</v>
       </c>
-      <c r="J20" s="35"/>
-    </row>
-    <row r="21" spans="2:10" s="31" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C21" s="1" t="s">
         <v>73</v>
       </c>
@@ -2826,9 +2852,8 @@
       <c r="I21" s="51" t="s">
         <v>199</v>
       </c>
-      <c r="J21" s="35"/>
-    </row>
-    <row r="22" spans="2:10" s="31" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="2:9" ht="63" x14ac:dyDescent="0.25">
       <c r="C22" s="3" t="s">
         <v>75</v>
       </c>
@@ -2847,9 +2872,8 @@
       <c r="I22" s="51" t="s">
         <v>199</v>
       </c>
-      <c r="J22" s="35"/>
-    </row>
-    <row r="23" spans="2:10" s="31" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C23" s="3" t="s">
         <v>77</v>
       </c>
@@ -2868,9 +2892,8 @@
       <c r="I23" s="51" t="s">
         <v>199</v>
       </c>
-      <c r="J23" s="35"/>
-    </row>
-    <row r="24" spans="2:10" s="31" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="2:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C24" s="3" t="s">
         <v>79</v>
       </c>
@@ -2889,9 +2912,8 @@
       <c r="I24" s="51" t="s">
         <v>199</v>
       </c>
-      <c r="J24" s="35"/>
-    </row>
-    <row r="25" spans="2:10" s="31" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="2:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C25" s="3" t="s">
         <v>81</v>
       </c>
@@ -2910,9 +2932,8 @@
       <c r="I25" s="51" t="s">
         <v>199</v>
       </c>
-      <c r="J25" s="35"/>
-    </row>
-    <row r="26" spans="2:10" s="31" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C26" s="3" t="s">
         <v>83</v>
       </c>
@@ -2931,9 +2952,8 @@
       <c r="I26" s="51" t="s">
         <v>199</v>
       </c>
-      <c r="J26" s="35"/>
-    </row>
-    <row r="27" spans="2:10" s="31" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="2:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C27" s="3" t="s">
         <v>85</v>
       </c>
@@ -2952,9 +2972,8 @@
       <c r="I27" s="51" t="s">
         <v>199</v>
       </c>
-      <c r="J27" s="35"/>
-    </row>
-    <row r="28" spans="2:10" s="31" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C28" s="3" t="s">
         <v>87</v>
       </c>
@@ -2973,9 +2992,8 @@
       <c r="I28" s="51" t="s">
         <v>199</v>
       </c>
-      <c r="J28" s="35"/>
-    </row>
-    <row r="29" spans="2:10" s="31" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C29" s="3" t="s">
         <v>89</v>
       </c>
@@ -2994,9 +3012,8 @@
       <c r="I29" s="51" t="s">
         <v>199</v>
       </c>
-      <c r="J29" s="35"/>
-    </row>
-    <row r="30" spans="2:10" s="31" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="2:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C30" s="3" t="s">
         <v>91</v>
       </c>
@@ -3015,9 +3032,8 @@
       <c r="I30" s="51" t="s">
         <v>199</v>
       </c>
-      <c r="J30" s="35"/>
-    </row>
-    <row r="31" spans="2:10" s="31" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="2:9" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C31" s="5" t="s">
         <v>93</v>
       </c>
@@ -3036,28 +3052,24 @@
       <c r="I31" s="51" t="s">
         <v>199</v>
       </c>
-      <c r="J31" s="35"/>
-    </row>
-    <row r="32" spans="2:10" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E32" s="51"/>
-      <c r="G32" s="35"/>
       <c r="I32" s="51"/>
-      <c r="J32" s="35"/>
-    </row>
-    <row r="33" spans="2:10" s="31" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="32" t="s">
         <v>68</v>
       </c>
       <c r="E33" s="51" t="s">
         <v>175</v>
       </c>
-      <c r="G33" s="35"/>
       <c r="I33" s="51"/>
       <c r="J33" s="34" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="34" spans="2:10" s="31" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C34" s="1" t="s">
         <v>95</v>
       </c>
@@ -3065,11 +3077,9 @@
         <v>96</v>
       </c>
       <c r="E34" s="51"/>
-      <c r="G34" s="35"/>
       <c r="I34" s="51"/>
-      <c r="J34" s="35"/>
-    </row>
-    <row r="35" spans="2:10" s="31" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="2:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C35" s="3" t="s">
         <v>97</v>
       </c>
@@ -3077,11 +3087,9 @@
         <v>98</v>
       </c>
       <c r="E35" s="51"/>
-      <c r="G35" s="35"/>
       <c r="I35" s="51"/>
-      <c r="J35" s="35"/>
-    </row>
-    <row r="36" spans="2:10" s="31" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C36" s="3" t="s">
         <v>99</v>
       </c>
@@ -3089,11 +3097,9 @@
         <v>100</v>
       </c>
       <c r="E36" s="51"/>
-      <c r="G36" s="35"/>
       <c r="I36" s="51"/>
-      <c r="J36" s="35"/>
-    </row>
-    <row r="37" spans="2:10" s="31" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="2:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C37" s="3" t="s">
         <v>101</v>
       </c>
@@ -3101,11 +3107,9 @@
         <v>102</v>
       </c>
       <c r="E37" s="51"/>
-      <c r="G37" s="35"/>
       <c r="I37" s="51"/>
-      <c r="J37" s="35"/>
-    </row>
-    <row r="38" spans="2:10" s="31" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="2:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C38" s="3" t="s">
         <v>103</v>
       </c>
@@ -3113,11 +3117,9 @@
         <v>104</v>
       </c>
       <c r="E38" s="51"/>
-      <c r="G38" s="35"/>
       <c r="I38" s="51"/>
-      <c r="J38" s="35"/>
-    </row>
-    <row r="39" spans="2:10" s="31" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C39" s="3" t="s">
         <v>105</v>
       </c>
@@ -3125,11 +3127,9 @@
         <v>106</v>
       </c>
       <c r="E39" s="51"/>
-      <c r="G39" s="35"/>
       <c r="I39" s="51"/>
-      <c r="J39" s="35"/>
-    </row>
-    <row r="40" spans="2:10" s="31" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="2:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C40" s="3" t="s">
         <v>107</v>
       </c>
@@ -3137,11 +3137,9 @@
         <v>108</v>
       </c>
       <c r="E40" s="51"/>
-      <c r="G40" s="35"/>
       <c r="I40" s="51"/>
-      <c r="J40" s="35"/>
-    </row>
-    <row r="41" spans="2:10" s="31" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="2:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C41" s="3" t="s">
         <v>109</v>
       </c>
@@ -3149,11 +3147,9 @@
         <v>110</v>
       </c>
       <c r="E41" s="51"/>
-      <c r="G41" s="35"/>
       <c r="I41" s="51"/>
-      <c r="J41" s="35"/>
-    </row>
-    <row r="42" spans="2:10" s="31" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="2:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C42" s="3" t="s">
         <v>111</v>
       </c>
@@ -3161,11 +3157,9 @@
         <v>112</v>
       </c>
       <c r="E42" s="51"/>
-      <c r="G42" s="35"/>
       <c r="I42" s="51"/>
-      <c r="J42" s="35"/>
-    </row>
-    <row r="43" spans="2:10" s="31" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="2:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C43" s="3" t="s">
         <v>113</v>
       </c>
@@ -3173,11 +3167,9 @@
         <v>114</v>
       </c>
       <c r="E43" s="51"/>
-      <c r="G43" s="35"/>
       <c r="I43" s="51"/>
-      <c r="J43" s="35"/>
-    </row>
-    <row r="44" spans="2:10" s="31" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="2:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C44" s="3" t="s">
         <v>115</v>
       </c>
@@ -3185,11 +3177,9 @@
         <v>116</v>
       </c>
       <c r="E44" s="51"/>
-      <c r="G44" s="35"/>
       <c r="I44" s="51"/>
-      <c r="J44" s="35"/>
-    </row>
-    <row r="45" spans="2:10" s="31" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="2:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C45" s="3" t="s">
         <v>117</v>
       </c>
@@ -3197,11 +3187,9 @@
         <v>118</v>
       </c>
       <c r="E45" s="51"/>
-      <c r="G45" s="35"/>
       <c r="I45" s="51"/>
-      <c r="J45" s="35"/>
-    </row>
-    <row r="46" spans="2:10" s="31" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="2:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C46" s="3" t="s">
         <v>119</v>
       </c>
@@ -3209,11 +3197,9 @@
         <v>120</v>
       </c>
       <c r="E46" s="51"/>
-      <c r="G46" s="35"/>
       <c r="I46" s="51"/>
-      <c r="J46" s="35"/>
-    </row>
-    <row r="47" spans="2:10" s="31" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="2:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C47" s="3" t="s">
         <v>121</v>
       </c>
@@ -3221,11 +3207,9 @@
         <v>122</v>
       </c>
       <c r="E47" s="51"/>
-      <c r="G47" s="35"/>
       <c r="I47" s="51"/>
-      <c r="J47" s="35"/>
-    </row>
-    <row r="48" spans="2:10" s="31" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="2:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C48" s="3" t="s">
         <v>123</v>
       </c>
@@ -3233,11 +3217,9 @@
         <v>124</v>
       </c>
       <c r="E48" s="51"/>
-      <c r="G48" s="35"/>
       <c r="I48" s="51"/>
-      <c r="J48" s="35"/>
-    </row>
-    <row r="49" spans="2:10" s="31" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="2:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C49" s="3" t="s">
         <v>125</v>
       </c>
@@ -3245,11 +3227,9 @@
         <v>126</v>
       </c>
       <c r="E49" s="51"/>
-      <c r="G49" s="35"/>
       <c r="I49" s="51"/>
-      <c r="J49" s="35"/>
-    </row>
-    <row r="50" spans="2:10" s="31" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="2:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C50" s="3" t="s">
         <v>127</v>
       </c>
@@ -3257,11 +3237,9 @@
         <v>128</v>
       </c>
       <c r="E50" s="51"/>
-      <c r="G50" s="35"/>
       <c r="I50" s="51"/>
-      <c r="J50" s="35"/>
-    </row>
-    <row r="51" spans="2:10" s="31" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="2:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C51" s="3" t="s">
         <v>129</v>
       </c>
@@ -3269,11 +3247,9 @@
         <v>130</v>
       </c>
       <c r="E51" s="51"/>
-      <c r="G51" s="35"/>
       <c r="I51" s="51"/>
-      <c r="J51" s="35"/>
-    </row>
-    <row r="52" spans="2:10" s="31" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C52" s="3" t="s">
         <v>131</v>
       </c>
@@ -3281,11 +3257,9 @@
         <v>132</v>
       </c>
       <c r="E52" s="51"/>
-      <c r="G52" s="35"/>
       <c r="I52" s="51"/>
-      <c r="J52" s="35"/>
-    </row>
-    <row r="53" spans="2:10" s="31" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="2:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C53" s="3" t="s">
         <v>133</v>
       </c>
@@ -3293,11 +3267,9 @@
         <v>134</v>
       </c>
       <c r="E53" s="51"/>
-      <c r="G53" s="35"/>
       <c r="I53" s="51"/>
-      <c r="J53" s="35"/>
-    </row>
-    <row r="54" spans="2:10" s="31" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="54" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C54" s="5" t="s">
         <v>135</v>
       </c>
@@ -3305,23 +3277,17 @@
         <v>136</v>
       </c>
       <c r="E54" s="51"/>
-      <c r="G54" s="35"/>
       <c r="I54" s="51"/>
-      <c r="J54" s="35"/>
-    </row>
-    <row r="55" spans="2:10" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E55" s="51"/>
-      <c r="G55" s="35"/>
       <c r="I55" s="51"/>
-      <c r="J55" s="35"/>
-    </row>
-    <row r="56" spans="2:10" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E56" s="51"/>
-      <c r="G56" s="35"/>
       <c r="I56" s="51"/>
-      <c r="J56" s="35"/>
-    </row>
-    <row r="57" spans="2:10" s="31" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="2:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B57" s="32" t="s">
         <v>65</v>
       </c>
@@ -3334,7 +3300,6 @@
       <c r="F57" s="32" t="s">
         <v>266</v>
       </c>
-      <c r="G57" s="35"/>
       <c r="H57" s="32" t="s">
         <v>198</v>
       </c>
@@ -3345,7 +3310,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="58" spans="2:10" s="31" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B58" s="32" t="s">
         <v>69</v>
       </c>
@@ -3358,7 +3323,6 @@
       <c r="F58" s="32" t="s">
         <v>271</v>
       </c>
-      <c r="G58" s="35"/>
       <c r="H58" s="32" t="s">
         <v>198</v>
       </c>
@@ -3369,7 +3333,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="59" spans="2:10" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B59" s="32" t="s">
         <v>71</v>
       </c>
@@ -3382,16 +3346,14 @@
       <c r="F59" s="32" t="s">
         <v>272</v>
       </c>
-      <c r="G59" s="35"/>
       <c r="H59" s="32" t="s">
         <v>198</v>
       </c>
       <c r="I59" s="51" t="s">
         <v>199</v>
       </c>
-      <c r="J59" s="35"/>
-    </row>
-    <row r="60" spans="2:10" s="31" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="2:10" ht="45" x14ac:dyDescent="0.25">
       <c r="C60" s="32" t="s">
         <v>176</v>
       </c>
@@ -3414,7 +3376,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="61" spans="2:10" s="31" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:10" ht="120" x14ac:dyDescent="0.25">
       <c r="C61" s="32" t="s">
         <v>208</v>
       </c>
@@ -3437,7 +3399,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="62" spans="2:10" s="31" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:10" ht="45" x14ac:dyDescent="0.25">
       <c r="C62" s="32" t="s">
         <v>182</v>
       </c>
@@ -3460,7 +3422,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="63" spans="2:10" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C63" s="32" t="s">
         <v>217</v>
       </c>
@@ -3479,9 +3441,8 @@
       <c r="I63" s="51" t="s">
         <v>199</v>
       </c>
-      <c r="J63" s="35"/>
-    </row>
-    <row r="64" spans="2:10" s="31" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="2:10" ht="135" x14ac:dyDescent="0.25">
       <c r="C64" s="32" t="s">
         <v>221</v>
       </c>
@@ -3500,9 +3461,8 @@
       <c r="I64" s="51" t="s">
         <v>199</v>
       </c>
-      <c r="J64" s="35"/>
-    </row>
-    <row r="65" spans="3:10" s="31" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="3:10" ht="60" x14ac:dyDescent="0.25">
       <c r="C65" s="32" t="s">
         <v>192</v>
       </c>
@@ -4130,8 +4090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{669A8674-0CB3-4109-94BC-90E1E61A8E33}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView topLeftCell="E10" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16:J24"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4331,7 +4291,9 @@
       </c>
     </row>
     <row r="13" spans="1:10" s="46" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="39"/>
+      <c r="A13" s="39" t="s">
+        <v>337</v>
+      </c>
       <c r="B13" s="9" t="s">
         <v>42</v>
       </c>
@@ -4353,7 +4315,9 @@
       </c>
     </row>
     <row r="14" spans="1:10" s="46" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="39"/>
+      <c r="A14" s="39" t="s">
+        <v>228</v>
+      </c>
       <c r="B14" s="9" t="s">
         <v>43</v>
       </c>
@@ -4373,7 +4337,9 @@
       </c>
     </row>
     <row r="15" spans="1:10" s="46" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="39"/>
+      <c r="A15" s="9" t="s">
+        <v>338</v>
+      </c>
       <c r="B15" s="9" t="s">
         <v>44</v>
       </c>
@@ -4605,7 +4571,9 @@
       </c>
     </row>
     <row r="25" spans="1:10" ht="63" x14ac:dyDescent="0.25">
-      <c r="A25" s="9"/>
+      <c r="A25" s="9" t="s">
+        <v>337</v>
+      </c>
       <c r="B25" s="9" t="s">
         <v>169</v>
       </c>
@@ -4633,7 +4601,9 @@
       <c r="J25" s="24"/>
     </row>
     <row r="26" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="9"/>
+      <c r="A26" s="9" t="s">
+        <v>337</v>
+      </c>
       <c r="B26" s="9"/>
       <c r="C26" s="24" t="s">
         <v>24</v>
@@ -4715,7 +4685,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8889FD6E-BB17-4303-8DB1-B0771B2ED0EC}">
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>

</xml_diff>